<commit_message>
Studied wrapcols and wraprows
</commit_message>
<xml_diff>
--- a/Momo-FillNonX.xlsx
+++ b/Momo-FillNonX.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EFD4AC4-4A24-417F-91DD-CD297ECEBF44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85277748-9810-40E3-887F-F8DDEDEF6A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7670ABE3-302C-455B-BF20-B006F3FAE6C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{7670ABE3-302C-455B-BF20-B006F3FAE6C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$5:$F$49</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -87,8 +91,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +121,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF009242"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF7030A0"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="3"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000099"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +206,19 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -167,11 +241,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -189,13 +300,114 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="13">
+    <cellStyle name="20% - Accent1 2" xfId="12" xr:uid="{7FDAB94F-38AC-412B-A60E-D0F47188B6FB}"/>
     <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="20% - Accent3 2" xfId="4" xr:uid="{DAC6F48D-BC2F-4294-9A03-7B8D7A9D9928}"/>
+    <cellStyle name="Comment" xfId="9" xr:uid="{58F59449-F115-4EA3-89DD-8DCA4342C967}"/>
+    <cellStyle name="Explanatory Text 2" xfId="6" xr:uid="{05979ACF-6848-4976-9C71-A27D2326D499}"/>
+    <cellStyle name="Heading 1 2" xfId="5" xr:uid="{BCEA0C40-E78A-4CEF-B9AC-254F1B26AD57}"/>
+    <cellStyle name="Heading 2 2" xfId="11" xr:uid="{19088E9D-26A3-4EFD-B3B1-AAC93E0D89BC}"/>
+    <cellStyle name="Heading 3 2" xfId="10" xr:uid="{07F448D5-87FB-41D2-9C14-8BE733D0EC5E}"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="8" xr:uid="{0C9D843D-1F39-4FCF-9910-2867C695A61F}"/>
+    <cellStyle name="Input 2" xfId="7" xr:uid="{A7E633F3-2CF9-4A20-B3DB-A932D174376F}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{AAD550FE-22E1-4D84-B0DE-7818AB0074E9}"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEAEAEA"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <bottom/>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <top style="double">
+          <color auto="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="double">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Biegert Standard" table="0" count="4" xr9:uid="{8298EBEA-8930-4495-AE67-59762960F1F6}">
+      <tableStyleElement type="headerRow" dxfId="7"/>
+      <tableStyleElement type="totalRow" dxfId="6"/>
+      <tableStyleElement type="firstColumn" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+    </tableStyle>
+    <tableStyle name="Biegert Standard A" pivot="0" count="4" xr9:uid="{B57BC1A2-48D0-4303-8D21-30452F780D07}">
+      <tableStyleElement type="headerRow" dxfId="3"/>
+      <tableStyleElement type="totalRow" dxfId="2"/>
+      <tableStyleElement type="firstColumn" dxfId="1"/>
+      <tableStyleElement type="firstRowStripe" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -589,7 +801,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5EEAB9-E28B-4013-B5B2-38620AA84DB0}">
   <dimension ref="A1:AM117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView topLeftCell="Q13" workbookViewId="0">
       <selection activeCell="AG29" sqref="AF29:AG29"/>
     </sheetView>
   </sheetViews>
@@ -2752,4 +2964,112 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C0818A-8E34-48A6-B1C6-F577805BCF0E}">
+  <dimension ref="B4:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="D5" cm="1">
+        <f t="array" ref="D5:F7">_xlfn.WRAPCOLS(B5:B11,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>7</v>
+      </c>
+      <c r="H5" cm="1">
+        <f t="array" ref="H5:J7">_xlfn.WRAPROWS(B5:B11,3,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>7</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>